<commit_message>
Graphe IA, rédaction des justifications, chiffrier excel pour la construction du graphe.
</commit_message>
<xml_diff>
--- a/DM2/ia.xlsx
+++ b/DM2/ia.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>I</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>reservation</t>
+  </si>
+  <si>
+    <t>payment</t>
   </si>
   <si>
     <t>usersessions</t>
@@ -249,10 +253,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.5</c:v>
                 </c:pt>
@@ -263,7 +267,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42857142857142855</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.5</c:v>
@@ -275,17 +279,20 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.25</c:v>
                 </c:pt>
@@ -305,10 +312,13 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,11 +591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142882032"/>
-        <c:axId val="142884384"/>
+        <c:axId val="444916824"/>
+        <c:axId val="444917216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142882032"/>
+        <c:axId val="444916824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -695,12 +705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142884384"/>
+        <c:crossAx val="444917216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142884384"/>
+        <c:axId val="444917216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -809,7 +819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142882032"/>
+        <c:crossAx val="444916824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -850,11 +860,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1414,25 +1419,29 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1445,7 +1454,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1714,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,26 +1824,26 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <f>D5/(E5+D5)</f>
-        <v>0.42857142857142855</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="C5">
         <f>F5/G5</f>
         <v>0.25</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1848,7 +1857,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <f>D6/(E6+D6)</f>
@@ -1873,7 +1882,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <f>D7/(E7+D7)</f>
@@ -1898,7 +1907,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <f>D8/(E8+D8)</f>
@@ -1906,7 +1915,7 @@
       </c>
       <c r="C8">
         <f>F8/G8</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1915,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -1923,18 +1932,18 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <f>D9/(E9+D9)</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C9">
         <f>F9/G9</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1946,19 +1955,42 @@
         <v>1</v>
       </c>
       <c r="V9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Y9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>D10/(E10+D10)</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>F10/G10</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
       <c r="V10">
         <v>0</v>
       </c>
@@ -2048,6 +2080,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
matin dimanche, changement d'ordi car version qui chie de vpp
</commit_message>
<xml_diff>
--- a/DM2/ia.xlsx
+++ b/DM2/ia.xlsx
@@ -264,13 +264,13 @@
                   <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -591,11 +591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="444916824"/>
-        <c:axId val="444917216"/>
+        <c:axId val="136096848"/>
+        <c:axId val="136097632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="444916824"/>
+        <c:axId val="136096848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -705,12 +705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="444917216"/>
+        <c:crossAx val="136097632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="444917216"/>
+        <c:axId val="136097632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -819,7 +819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="444916824"/>
+        <c:crossAx val="136096848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,15 +1810,15 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <f>D4/(E4+D4)</f>
-        <v>0.5</v>
+        <f t="shared" ref="B4:B10" si="2">D4/(E4+D4)</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C4">
-        <f>F4/G4</f>
+        <f t="shared" ref="C4:C10" si="3">F4/G4</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1835,18 +1835,18 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <f>D5/(E5+D5)</f>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C5">
-        <f>F5/G5</f>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1860,15 +1860,15 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <f>D6/(E6+D6)</f>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <f>F6/G6</f>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1885,11 +1885,11 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>D7/(E7+D7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C7">
-        <f>F7/G7</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="D7">
@@ -1910,11 +1910,11 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <f>D8/(E8+D8)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C8">
-        <f>F8/G8</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="D8">
@@ -1935,11 +1935,11 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <f>D9/(E9+D9)</f>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="C9">
-        <f>F9/G9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D9">
@@ -1972,11 +1972,11 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <f>D10/(E10+D10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>F10/G10</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="D10">

</xml_diff>